<commit_message>
Reorganización completa: limpieza de módulos antiguos, nuevas entregas y optimización
</commit_message>
<xml_diff>
--- a/plantillas de carga/plantilla_animales.xlsx
+++ b/plantillas de carga/plantilla_animales.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="animales" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,24 +25,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -57,11 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,159 +413,108 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
-    <col width="20" customWidth="1" min="10" max="10"/>
-    <col width="20" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="20" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="20" customWidth="1" min="15" max="15"/>
-    <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="20" customWidth="1" min="17" max="17"/>
-    <col width="20" customWidth="1" min="18" max="18"/>
-    <col width="20" customWidth="1" min="19" max="19"/>
-    <col width="20" customWidth="1" min="20" max="20"/>
-    <col width="20" customWidth="1" min="21" max="21"/>
-    <col width="20" customWidth="1" min="22" max="22"/>
-    <col width="20" customWidth="1" min="23" max="23"/>
-    <col width="20" customWidth="1" min="24" max="24"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Código</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo Ingreso</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Sexo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha Nacimiento</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha Compra</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Finca</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Raza</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Potrero</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Lote</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Sector</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Grupo</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Peso Nacimiento</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Peso Compra</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Precio Compra</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Vendedor</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Procedencia</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Salud</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Inventariado</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Color</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Hierro</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Condición Corporal</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Comentario</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>codigo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>tipo_ingreso</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>sexo</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fecha_nacimiento</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fecha_compra</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>finca</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>raza</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>potrero</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>peso_nacimiento</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>peso_compra</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>precio_compra</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>salud</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>inventariado</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>hierro</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>condicion_corporal</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>comentario</t>
         </is>
       </c>
     </row>

</xml_diff>